<commit_message>
refactor(ld46) rename some effects
</commit_message>
<xml_diff>
--- a/packages/ld46/docs/cards/Actions.xlsx
+++ b/packages/ld46/docs/cards/Actions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\jou\packages\ld46\docs\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09841F0-D049-4396-9625-C87884766D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF77235-5168-40AF-9D0F-686E6FBCE103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="1215" windowWidth="19155" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>action_template.png</t>
   </si>
@@ -211,6 +211,19 @@
   </si>
   <si>
     <t>+5 Excitement for the player</t>
+  </si>
+  <si>
+    <t>Sacrifice</t>
+  </si>
+  <si>
+    <t>Sacrifice Self</t>
+  </si>
+  <si>
+    <t>The gladiator throws themselves in front of the opponent, saving their comrades.</t>
+  </si>
+  <si>
+    <t>The fighter is discarded
+Targeted creature cannot attack</t>
   </si>
 </sst>
 </file>
@@ -536,13 +549,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,6 +924,38 @@
         <v>54</v>
       </c>
     </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>